<commit_message>
Se agregó folio, validación y limpieza de datos y se cambió la imagen.
</commit_message>
<xml_diff>
--- a/Base General.xlsx
+++ b/Base General.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="24260" windowHeight="13740" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,6 +26,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -418,20 +419,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="29.33203125" customWidth="1" min="1" max="1"/>
-    <col width="11.77734375" customWidth="1" min="2" max="2"/>
-    <col width="12.44140625" customWidth="1" min="3" max="3"/>
-    <col width="40.44140625" customWidth="1" min="4" max="4"/>
-    <col width="27.88671875" customWidth="1" min="5" max="5"/>
-    <col width="11.21875" customWidth="1" min="6" max="6"/>
+    <col width="11.83203125" customWidth="1" min="2" max="2"/>
+    <col width="12.5" customWidth="1" min="3" max="3"/>
+    <col width="40.5" customWidth="1" min="4" max="4"/>
+    <col width="27.83203125" customWidth="1" min="5" max="5"/>
+    <col width="11.1640625" customWidth="1" min="6" max="6"/>
     <col width="9.6640625" customWidth="1" min="8" max="8"/>
     <col width="13.33203125" customWidth="1" min="9" max="9"/>
   </cols>
@@ -469,12 +470,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Turno</t>
+          <t>Hora</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Hora</t>
+          <t>Folio</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -486,269 +487,94 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alex Serrano Durán</t>
+          <t>ALEX SERRANO DURÁN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>55 63193656</t>
+          <t>5563193656</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>alexserrano0805@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>52950</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>alexserrano0805@gmail.com</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Consulta</t>
+          <t>CONSULTA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>$600</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>04:24</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0:56</t>
+          <t>000-20220825M</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>13/7/2022</t>
+          <t>26/08/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alex Serrano</t>
+          <t>ALEX SERRANO DURÁN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>55 63193656</t>
+          <t>5563193656</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>alexserrano0805@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>52950</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>alexserrano0805@gmail.com</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Consulta</t>
+          <t>CONSULTA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>$400</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>04:26</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>15:7</t>
+          <t>001-20220825N</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>13/7/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Seleccionar</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0:19</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>15/7/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Alex Serrano</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>55 63193656</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>alexserrano0805@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>52950</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Consulta</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Seleccionar</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>19:55</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>18/7/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Seleccionar</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>20:29</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>18/07/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Alex Serrano Durán</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>55 63193656</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>alexserrano0805@gmail.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>52950</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Consulta</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Vespertino</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>21:07</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>18/07/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Alex Serrano</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>55 63193656</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>alexserrano0805@gmail.com</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>52950</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Consulta</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>600.00</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Vespertino</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>21:23</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>18/07/2022</t>
+          <t>26/08/2022</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregó el tipo de pago, nuevo formato para corte de caja y se reparó error donde la fecha en el folio no tomaba en cuenta el turno de madrugada
</commit_message>
<xml_diff>
--- a/Base General.xlsx
+++ b/Base General.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -51,9 +53,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,21 +423,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="29.33203125" customWidth="1" min="1" max="1"/>
+    <col width="34.83203125" customWidth="1" min="1" max="1"/>
     <col width="11.83203125" customWidth="1" min="2" max="2"/>
-    <col width="12.5" customWidth="1" min="3" max="3"/>
-    <col width="40.5" customWidth="1" min="4" max="4"/>
-    <col width="27.83203125" customWidth="1" min="5" max="5"/>
-    <col width="11.1640625" customWidth="1" min="6" max="6"/>
-    <col width="9.6640625" customWidth="1" min="8" max="8"/>
+    <col width="34.5" customWidth="1" min="3" max="3"/>
+    <col width="14.83203125" customWidth="1" min="4" max="4"/>
+    <col width="34" customWidth="1" min="5" max="5"/>
+    <col width="17.5" customWidth="1" style="3" min="6" max="6"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
     <col width="13.33203125" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
@@ -450,20 +454,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Correo Electrónico</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Código Postal</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Correo Electrónico</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Servicio</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Importe</t>
         </is>
@@ -510,7 +514,7 @@
           <t>CONSULTA</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>$600</t>
         </is>
@@ -557,7 +561,7 @@
           <t>CONSULTA</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>$400</t>
         </is>
@@ -575,6 +579,387 @@
       <c r="I3" t="inlineStr">
         <is>
           <t>26/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ALEX SERRANO DURÁN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5563193656</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>alexserrano0805@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>52950</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CONSULTA</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>$600</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>001-20220826M</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>26/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5563193656</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>mmm@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01022</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>$600.50</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>002-20220826M</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>26/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>555</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>alex@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3333</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>$600</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>12:11</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>001-20220826V</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>26/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ALEX</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>556214</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>124124</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>$600</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>003-20220826M</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>26/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ALEX SERRANO</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>123123123</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>alexserrano0805</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>125521</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>$123</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>02:28</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>001-20220827V</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>28/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12312312</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>aaqa@.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>52950</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Efectivo</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>02:53</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>001-20220827N</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>28/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>556219305</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>aaa@.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15252</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Efectivo</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>03:02</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>28/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5516169339</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>aaa@a.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15154</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>03:13</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>003-20220827N</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>27/08/2022</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se creó el formato de Excel para el Corte de Caja y se remodeló la ventana de UI
</commit_message>
<xml_diff>
--- a/Base General.xlsx
+++ b/Base General.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -963,6 +963,617 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NOMBRE PRUEBA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>12313287</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>bbb@b.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>09216</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SERVICIO PRUEBA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>03:21</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>001-20220827N</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>27/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PRUEBA EFE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>3123121239</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>aaa@efe.com</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>09127</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>PRUEBA EFE</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>03:26</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>001-20220827V</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>27/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>OLA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5563191314</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>das@sad.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>76123</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>COMO ESTAS</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>01:58</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>007-20220829N</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ALEX SERRANO DURAN</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12386709</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>alexserrano@hu.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>67354</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CONSULTA</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1283913892</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>aaa@com</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>53478</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>$412</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>04:22</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NOMBRE</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>3475890123</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>aaa@com</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>35764</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>$123</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>04:24</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2438708132</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>aaa@.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>91323</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>PRUEBA CELDAS UNIDAS</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>$213</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>04:27</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0157378645</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>aaa@c.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>97246</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>PRUEBA ANCHO COLUMNAS</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>$531</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>04:35</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>002-20220829N</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>9248751248</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>aaa@a.com</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>51387</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>PRUEBAANCHO 2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>$931</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>04:39</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>003-20220829N</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3891281241</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>aaa@a.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>11329</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>PRUEBA ANCHO 3</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>$132</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>04:40</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>7831257236</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>aaa@qa.com</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>18294</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>PRUEBA ANCHO FINAL(ESPERO)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>$567</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>04:41</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>9183262843</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>alex@gmail.com</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>90132</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>PRUEBA ANCHO FINAL ORASI</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>$247</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>04:43</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>002-20220829N</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ALEX SERRANO</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1937504826</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>alex@gmi.com</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>82735</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>PRUEBÍSIMA FINAL ANCHO</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>$824</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>04:44</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>001-20220829N</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>29/08/2022</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Creación e impresión de documento lista
</commit_message>
<xml_diff>
--- a/Base General.xlsx
+++ b/Base General.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="24260" windowHeight="13740" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1668,6 +1668,382 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ELIABET VARELA REYES</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1212126556</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>eliabetvarela@gmail.com</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>13589</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CONSULTA</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>001-20220906V</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PRUEBA LANDSCAPE</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1238923154</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>aaa@.com</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>13223</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>$132</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>002-20220906V</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>TEST LANDSCAPE</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>12312321</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>aaa@.com</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>12378</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>CONSULTA</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>$123</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>18:07</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>003-20220906V</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>TESTDOCUMENTLANDSCAPE</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>12332</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>SERVICIO|</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>$1</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>18:09</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>004-20220906V</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CARLOS PEÑA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>213712373127</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>cpena@gmail.com</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>31265</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>CONSULTA</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>$300</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>18:12</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>005-20220906V</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>213132123</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>correo</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>12323</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>04:41</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>001-20220906N</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2132345454</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>correo</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>21323</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>04:43</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>001-20220906M</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PRUEBA CARPETAS</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2183981233</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>98123</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>$300</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>001-20220906V</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>06/09/2022</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>